<commit_message>
Naive cost calculations for modafinil.
</commit_message>
<xml_diff>
--- a/_Modafinil/Route_4.xlsx
+++ b/_Modafinil/Route_4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mseifrid/Dropbox (Aspuru-Guzik Lab)/Matter Lab/Data/Code/Chemical subway/RouteScore_preprint/modafinil/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mseifrid/Dropbox (Aspuru-Guzik Lab)/Matter Lab/Data/Code/Subway_Maps/_Modafinil/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1B134E-FD24-EF49-B783-B96DBFF9D024}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DB0DCD-0636-9844-B00D-FC3C687486D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{452BDC74-8E04-244A-8FD4-DEB31974EB7F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="2" xr2:uid="{452BDC74-8E04-244A-8FD4-DEB31974EB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Step 1" sheetId="1" r:id="rId1"/>
@@ -550,7 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B591C0B3-C972-1249-ACD8-05DFA8EA3DB3}">
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AH13" sqref="AH13"/>
     </sheetView>
   </sheetViews>
@@ -1001,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C724923E-52E7-FA4F-A5A5-ABFC7A2E6BDF}">
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1:Z1048576"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1130,7 +1130,7 @@
       </c>
       <c r="S2">
         <f>SUM(K2:K12)+N2*O2</f>
-        <v>88.283333335099002</v>
+        <v>88.801143244996467</v>
       </c>
       <c r="T2">
         <f>SUM(L2:L12)</f>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="X2">
         <f>S2/Y2</f>
-        <v>15793.082886422006</v>
+        <v>15885.71435509776</v>
       </c>
       <c r="Y2">
         <f>P2*MIN(H2:H6)</f>
@@ -1152,7 +1152,7 @@
       </c>
       <c r="Z2">
         <f>R2*S2*T2</f>
-        <v>492.2605097419127</v>
+        <v>495.14777464873288</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -1183,6 +1183,10 @@
       </c>
       <c r="I3" t="s">
         <v>48</v>
+      </c>
+      <c r="K3">
+        <f>H3*G3</f>
+        <v>0.51780990989747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>